<commit_message>
Day 11 - DQL - Pre-lunch
</commit_message>
<xml_diff>
--- a/Day 10/Normalized Emptable.xlsx
+++ b/Day 10/Normalized Emptable.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\OneDrive\Desktop\EY 24\E-Y-Induction-24\Day 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63AD0AC-A0B4-4F6B-8DF9-9B1BA660CF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AABED3-78DB-45D8-88DB-8784D9C67E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="1" xr2:uid="{57A09CD9-A068-4F39-8AB6-A97CB8F2008B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{57A09CD9-A068-4F39-8AB6-A97CB8F2008B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="49">
   <si>
     <t>EmpNo</t>
   </si>
@@ -172,6 +173,18 @@
   </si>
   <si>
     <t>PassengerInfo</t>
+  </si>
+  <si>
+    <t>DeptName</t>
+  </si>
+  <si>
+    <t>EmpDesignation</t>
+  </si>
+  <si>
+    <t>deptNo</t>
+  </si>
+  <si>
+    <t>empDeptNo</t>
   </si>
 </sst>
 </file>
@@ -650,6 +663,65 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>506185</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>103414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connector: Elbow 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E3B945-2015-9E38-F65C-6CACD330D569}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="506185" y="103414"/>
+          <a:ext cx="7119258" cy="1083129"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1416,7 +1488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27065BA1-A135-4572-8918-7B09F6D964B9}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16:M18"/>
     </sheetView>
   </sheetViews>
@@ -1957,4 +2029,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A298A6B-AD5B-4296-A526-3008112D1A9B}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.07421875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A3" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A4" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A5" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="L11" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="L13" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="L15" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="L16" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="8:12" x14ac:dyDescent="0.4">
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="L17" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12" x14ac:dyDescent="0.4">
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="L18" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12" x14ac:dyDescent="0.4">
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="L19" s="3">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DML - Joins - Morequeries
</commit_message>
<xml_diff>
--- a/Day 10/Normalized Emptable.xlsx
+++ b/Day 10/Normalized Emptable.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\OneDrive\Desktop\EY 24\E-Y-Induction-24\Day 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487CDF2F-F153-4C9A-9ED7-3954C285F46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F825FF-A7FF-43DE-BEDD-C05A1F03BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{57A09CD9-A068-4F39-8AB6-A97CB8F2008B}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="3" xr2:uid="{57A09CD9-A068-4F39-8AB6-A97CB8F2008B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="54">
   <si>
     <t>EmpNo</t>
   </si>
@@ -172,9 +173,6 @@
     <t>FlightSchedule Table</t>
   </si>
   <si>
-    <t>PassengerInfo</t>
-  </si>
-  <si>
     <t>DeptName</t>
   </si>
   <si>
@@ -185,6 +183,24 @@
   </si>
   <si>
     <t>empDeptNo</t>
+  </si>
+  <si>
+    <t>Mellissia</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Sampath</t>
+  </si>
+  <si>
+    <t>Nainesh</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -663,6 +679,196 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AF1F634-83C1-8437-BAEC-B3341F7D1B95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3929743" y="185057"/>
+          <a:ext cx="2122714" cy="70757"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>70757</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>146957</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A99E66E-2691-B42E-B6F8-3534A00A89A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4495801" y="1736271"/>
+          <a:ext cx="3799113" cy="1213757"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>DeptNo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
+            <a:t> will be allocated once the finish the training after 40 days</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" baseline="0"/>
+            <a:t>based on their performance and vacancy in department / projects after 40 days</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>642257</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>157843</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{707AC942-6AB8-26BF-76AA-2AA4E1155EDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4218214" y="2343150"/>
+          <a:ext cx="277587" cy="35379"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1430,7 +1636,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16:M18"/>
+      <selection activeCell="M15" sqref="M15:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1772,14 +1978,9 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B13" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B14">
-        <v>11</v>
-      </c>
       <c r="M14" t="s">
         <v>34</v>
       </c>
@@ -1976,7 +2177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A298A6B-AD5B-4296-A526-3008112D1A9B}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9:M19"/>
     </sheetView>
   </sheetViews>
@@ -1989,10 +2190,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -2040,13 +2241,13 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.4">
@@ -2132,4 +2333,451 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A155BF-3BDE-4E16-8E04-9C78CD4820C3}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="13.61328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5">
+        <v>16255</v>
+      </c>
+      <c r="E2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="5">
+        <v>18454</v>
+      </c>
+      <c r="E3" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12950</v>
+      </c>
+      <c r="E4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3">
+        <v>30</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5">
+        <v>22817</v>
+      </c>
+      <c r="E5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5813</v>
+      </c>
+      <c r="E6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9704</v>
+      </c>
+      <c r="E7" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <v>11956</v>
+      </c>
+      <c r="E8" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="5">
+        <v>24941</v>
+      </c>
+      <c r="E9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="5">
+        <v>16655</v>
+      </c>
+      <c r="E10" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="5">
+        <v>21044</v>
+      </c>
+      <c r="E11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E12" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E15" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4000</v>
+      </c>
+      <c r="E16" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>